<commit_message>
methylseq statistics and WGBS output
</commit_message>
<xml_diff>
--- a/Dec-July-2019-analysis/output/statistics/Results_summary.xlsx
+++ b/Dec-July-2019-analysis/output/statistics/Results_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/Dec-July-2019-analysis/output/statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3262D5-0193-7140-B88D-44EE94269777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51E9320-154F-344A-8126-C6A6649EB53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6340" yWindow="700" windowWidth="27240" windowHeight="19560" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3038,7 +3038,7 @@
   <dimension ref="B1:K50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>